<commit_message>
adding back low values as LLOQ/2 as suggested by Nestlé
</commit_message>
<xml_diff>
--- a/LGC_Motiv_results/study1/blood_NAD/20221114_CS_Final_Complete_Baseline_Summary_shared_CSTeam_sent.xlsx
+++ b/LGC_Motiv_results/study1/blood_NAD/20221114_CS_Final_Complete_Baseline_Summary_shared_CSTeam_sent.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RDMeisseKa\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Loco\Documents\GitHub\LGC_motiv\LGC_Motiv_results\study1\blood_NAD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B2914514-B610-4D82-94DD-24E2315DDE49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23609909-427D-4543-BCCC-BA779B1051F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14730" yWindow="1500" windowWidth="13635" windowHeight="9810" tabRatio="277" xr2:uid="{F62A85C5-58E9-4FF9-A043-57519E2747BB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="277" xr2:uid="{F62A85C5-58E9-4FF9-A043-57519E2747BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Final" sheetId="5" r:id="rId1"/>
@@ -371,7 +371,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -416,7 +416,7 @@
       <name val="Nestle Text TF VN Book Cnd"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -426,6 +426,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -504,7 +510,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -568,6 +574,9 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -588,7 +597,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -887,11 +896,11 @@
   <dimension ref="A1:N103"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J96" sqref="J96"/>
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P37" sqref="P37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.28515625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
@@ -901,7 +910,7 @@
     <col min="15" max="15" width="3.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" ht="18.75" thickBot="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -940,7 +949,7 @@
       </c>
       <c r="M1" s="1"/>
     </row>
-    <row r="2" spans="1:13" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" ht="18">
       <c r="A2" s="6"/>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -955,7 +964,7 @@
       <c r="L2" s="7"/>
       <c r="M2" s="1"/>
     </row>
-    <row r="3" spans="1:13" ht="18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" ht="18">
       <c r="A3" s="9" t="s">
         <v>82</v>
       </c>
@@ -1005,7 +1014,7 @@
       </c>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="1:13" ht="18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" ht="18">
       <c r="A4" s="9" t="s">
         <v>83</v>
       </c>
@@ -1053,7 +1062,7 @@
       </c>
       <c r="M4" s="1"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -1068,7 +1077,7 @@
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
     </row>
-    <row r="6" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" s="16" customFormat="1">
       <c r="A6" s="12" t="s">
         <v>11</v>
       </c>
@@ -1109,7 +1118,7 @@
       </c>
       <c r="M6" s="15"/>
     </row>
-    <row r="7" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" s="16" customFormat="1">
       <c r="A7" s="12" t="s">
         <v>12</v>
       </c>
@@ -1150,7 +1159,7 @@
       </c>
       <c r="M7" s="15"/>
     </row>
-    <row r="8" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" s="16" customFormat="1">
       <c r="A8" s="12" t="s">
         <v>13</v>
       </c>
@@ -1191,7 +1200,7 @@
       </c>
       <c r="M8" s="15"/>
     </row>
-    <row r="9" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" s="16" customFormat="1">
       <c r="A9" s="12" t="s">
         <v>14</v>
       </c>
@@ -1232,7 +1241,7 @@
       </c>
       <c r="M9" s="15"/>
     </row>
-    <row r="10" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" s="16" customFormat="1">
       <c r="A10" s="12" t="s">
         <v>15</v>
       </c>
@@ -1273,7 +1282,7 @@
       </c>
       <c r="M10" s="15"/>
     </row>
-    <row r="11" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" s="16" customFormat="1">
       <c r="A11" s="12" t="s">
         <v>16</v>
       </c>
@@ -1314,7 +1323,7 @@
       </c>
       <c r="M11" s="15"/>
     </row>
-    <row r="12" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" s="16" customFormat="1">
       <c r="A12" s="12" t="s">
         <v>17</v>
       </c>
@@ -1355,7 +1364,7 @@
       </c>
       <c r="M12" s="15"/>
     </row>
-    <row r="13" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" s="16" customFormat="1">
       <c r="A13" s="12" t="s">
         <v>18</v>
       </c>
@@ -1396,7 +1405,7 @@
       </c>
       <c r="M13" s="15"/>
     </row>
-    <row r="14" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" s="16" customFormat="1">
       <c r="A14" s="12" t="s">
         <v>19</v>
       </c>
@@ -1437,7 +1446,7 @@
       </c>
       <c r="M14" s="15"/>
     </row>
-    <row r="15" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" s="16" customFormat="1">
       <c r="A15" s="12" t="s">
         <v>20</v>
       </c>
@@ -1478,7 +1487,7 @@
       </c>
       <c r="M15" s="15"/>
     </row>
-    <row r="16" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" s="16" customFormat="1">
       <c r="A16" s="12" t="s">
         <v>21</v>
       </c>
@@ -1497,7 +1506,7 @@
       <c r="F16" s="14">
         <v>0.72877091714912867</v>
       </c>
-      <c r="G16" s="14" t="s">
+      <c r="G16" s="23" t="s">
         <v>1</v>
       </c>
       <c r="H16" s="14">
@@ -1519,7 +1528,7 @@
       </c>
       <c r="M16" s="15"/>
     </row>
-    <row r="17" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" s="16" customFormat="1">
       <c r="A17" s="12" t="s">
         <v>22</v>
       </c>
@@ -1560,7 +1569,7 @@
       </c>
       <c r="M17" s="15"/>
     </row>
-    <row r="18" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" s="16" customFormat="1">
       <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
@@ -1601,7 +1610,7 @@
       </c>
       <c r="M18" s="15"/>
     </row>
-    <row r="19" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" s="16" customFormat="1">
       <c r="A19" s="12" t="s">
         <v>24</v>
       </c>
@@ -1642,7 +1651,7 @@
       </c>
       <c r="M19" s="15"/>
     </row>
-    <row r="20" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" s="16" customFormat="1">
       <c r="A20" s="12" t="s">
         <v>25</v>
       </c>
@@ -1683,7 +1692,7 @@
       </c>
       <c r="M20" s="15"/>
     </row>
-    <row r="21" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" s="16" customFormat="1">
       <c r="A21" s="12" t="s">
         <v>26</v>
       </c>
@@ -1724,7 +1733,7 @@
       </c>
       <c r="M21" s="15"/>
     </row>
-    <row r="22" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" s="16" customFormat="1">
       <c r="A22" s="12" t="s">
         <v>27</v>
       </c>
@@ -1765,7 +1774,7 @@
       </c>
       <c r="M22" s="15"/>
     </row>
-    <row r="23" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" s="16" customFormat="1">
       <c r="A23" s="12" t="s">
         <v>28</v>
       </c>
@@ -1806,7 +1815,7 @@
       </c>
       <c r="M23" s="15"/>
     </row>
-    <row r="24" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" s="16" customFormat="1">
       <c r="A24" s="12" t="s">
         <v>29</v>
       </c>
@@ -1847,7 +1856,7 @@
       </c>
       <c r="M24" s="15"/>
     </row>
-    <row r="25" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" s="16" customFormat="1">
       <c r="A25" s="12" t="s">
         <v>30</v>
       </c>
@@ -1888,7 +1897,7 @@
       </c>
       <c r="M25" s="15"/>
     </row>
-    <row r="26" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" s="16" customFormat="1">
       <c r="A26" s="12" t="s">
         <v>31</v>
       </c>
@@ -1929,7 +1938,7 @@
       </c>
       <c r="M26" s="15"/>
     </row>
-    <row r="27" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" s="16" customFormat="1">
       <c r="A27" s="12" t="s">
         <v>32</v>
       </c>
@@ -1970,7 +1979,7 @@
       </c>
       <c r="M27" s="15"/>
     </row>
-    <row r="28" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" s="16" customFormat="1">
       <c r="A28" s="12" t="s">
         <v>33</v>
       </c>
@@ -2011,7 +2020,7 @@
       </c>
       <c r="M28" s="15"/>
     </row>
-    <row r="29" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" s="16" customFormat="1">
       <c r="A29" s="12" t="s">
         <v>34</v>
       </c>
@@ -2052,7 +2061,7 @@
       </c>
       <c r="M29" s="15"/>
     </row>
-    <row r="30" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" s="16" customFormat="1">
       <c r="A30" s="12" t="s">
         <v>35</v>
       </c>
@@ -2093,7 +2102,7 @@
       </c>
       <c r="M30" s="15"/>
     </row>
-    <row r="31" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" s="16" customFormat="1">
       <c r="A31" s="12" t="s">
         <v>36</v>
       </c>
@@ -2134,7 +2143,7 @@
       </c>
       <c r="M31" s="15"/>
     </row>
-    <row r="32" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" s="16" customFormat="1">
       <c r="A32" s="12" t="s">
         <v>37</v>
       </c>
@@ -2175,7 +2184,7 @@
       </c>
       <c r="M32" s="15"/>
     </row>
-    <row r="33" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" s="16" customFormat="1">
       <c r="A33" s="12" t="s">
         <v>38</v>
       </c>
@@ -2197,7 +2206,7 @@
       <c r="G33" s="14">
         <v>0.11600000000000001</v>
       </c>
-      <c r="H33" s="14" t="s">
+      <c r="H33" s="23" t="s">
         <v>1</v>
       </c>
       <c r="I33" s="14">
@@ -2216,7 +2225,7 @@
       </c>
       <c r="M33" s="15"/>
     </row>
-    <row r="34" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" s="16" customFormat="1">
       <c r="A34" s="12" t="s">
         <v>39</v>
       </c>
@@ -2238,7 +2247,7 @@
       <c r="G34" s="14">
         <v>0.02</v>
       </c>
-      <c r="H34" s="14" t="s">
+      <c r="H34" s="23" t="s">
         <v>1</v>
       </c>
       <c r="I34" s="14">
@@ -2257,7 +2266,7 @@
       </c>
       <c r="M34" s="15"/>
     </row>
-    <row r="35" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" s="16" customFormat="1">
       <c r="A35" s="12" t="s">
         <v>40</v>
       </c>
@@ -2298,7 +2307,7 @@
       </c>
       <c r="M35" s="15"/>
     </row>
-    <row r="36" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" s="16" customFormat="1">
       <c r="A36" s="12" t="s">
         <v>41</v>
       </c>
@@ -2339,7 +2348,7 @@
       </c>
       <c r="M36" s="15"/>
     </row>
-    <row r="37" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" s="16" customFormat="1">
       <c r="A37" s="12" t="s">
         <v>42</v>
       </c>
@@ -2361,7 +2370,7 @@
       <c r="G37" s="14">
         <v>5.7000000000000002E-2</v>
       </c>
-      <c r="H37" s="14" t="s">
+      <c r="H37" s="23" t="s">
         <v>1</v>
       </c>
       <c r="I37" s="14">
@@ -2380,7 +2389,7 @@
       </c>
       <c r="M37" s="15"/>
     </row>
-    <row r="38" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" s="16" customFormat="1">
       <c r="A38" s="12" t="s">
         <v>43</v>
       </c>
@@ -2421,7 +2430,7 @@
       </c>
       <c r="M38" s="15"/>
     </row>
-    <row r="39" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" s="16" customFormat="1">
       <c r="A39" s="12" t="s">
         <v>44</v>
       </c>
@@ -2462,7 +2471,7 @@
       </c>
       <c r="M39" s="15"/>
     </row>
-    <row r="40" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" s="16" customFormat="1">
       <c r="A40" s="12" t="s">
         <v>45</v>
       </c>
@@ -2503,7 +2512,7 @@
       </c>
       <c r="M40" s="15"/>
     </row>
-    <row r="41" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" s="16" customFormat="1">
       <c r="A41" s="12" t="s">
         <v>46</v>
       </c>
@@ -2544,7 +2553,7 @@
       </c>
       <c r="M41" s="15"/>
     </row>
-    <row r="42" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" s="16" customFormat="1">
       <c r="A42" s="12" t="s">
         <v>47</v>
       </c>
@@ -2585,7 +2594,7 @@
       </c>
       <c r="M42" s="15"/>
     </row>
-    <row r="43" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" s="16" customFormat="1">
       <c r="A43" s="12" t="s">
         <v>48</v>
       </c>
@@ -2607,7 +2616,7 @@
       <c r="G43" s="14">
         <v>0.21</v>
       </c>
-      <c r="H43" s="14" t="s">
+      <c r="H43" s="23" t="s">
         <v>1</v>
       </c>
       <c r="I43" s="14">
@@ -2626,7 +2635,7 @@
       </c>
       <c r="M43" s="15"/>
     </row>
-    <row r="44" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" s="16" customFormat="1">
       <c r="A44" s="12" t="s">
         <v>49</v>
       </c>
@@ -2648,7 +2657,7 @@
       <c r="G44" s="14">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="H44" s="14" t="s">
+      <c r="H44" s="23" t="s">
         <v>1</v>
       </c>
       <c r="I44" s="14">
@@ -2667,7 +2676,7 @@
       </c>
       <c r="M44" s="15"/>
     </row>
-    <row r="45" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" s="16" customFormat="1">
       <c r="A45" s="12" t="s">
         <v>50</v>
       </c>
@@ -2689,7 +2698,7 @@
       <c r="G45" s="14">
         <v>4.7E-2</v>
       </c>
-      <c r="H45" s="14" t="s">
+      <c r="H45" s="23" t="s">
         <v>1</v>
       </c>
       <c r="I45" s="14">
@@ -2708,7 +2717,7 @@
       </c>
       <c r="M45" s="15"/>
     </row>
-    <row r="46" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" s="16" customFormat="1">
       <c r="A46" s="12" t="s">
         <v>51</v>
       </c>
@@ -2749,7 +2758,7 @@
       </c>
       <c r="M46" s="15"/>
     </row>
-    <row r="47" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" s="16" customFormat="1">
       <c r="A47" s="12" t="s">
         <v>52</v>
       </c>
@@ -2790,7 +2799,7 @@
       </c>
       <c r="M47" s="15"/>
     </row>
-    <row r="48" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" s="16" customFormat="1">
       <c r="A48" s="12" t="s">
         <v>53</v>
       </c>
@@ -2812,7 +2821,7 @@
       <c r="G48" s="14">
         <v>3.3000000000000002E-2</v>
       </c>
-      <c r="H48" s="14" t="s">
+      <c r="H48" s="23" t="s">
         <v>1</v>
       </c>
       <c r="I48" s="14">
@@ -2831,7 +2840,7 @@
       </c>
       <c r="M48" s="15"/>
     </row>
-    <row r="49" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" s="16" customFormat="1">
       <c r="A49" s="12" t="s">
         <v>54</v>
       </c>
@@ -2872,7 +2881,7 @@
       </c>
       <c r="M49" s="15"/>
     </row>
-    <row r="50" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" s="16" customFormat="1">
       <c r="A50" s="12" t="s">
         <v>55</v>
       </c>
@@ -2894,7 +2903,7 @@
       <c r="G50" s="14">
         <v>5.7000000000000002E-2</v>
       </c>
-      <c r="H50" s="14" t="s">
+      <c r="H50" s="23" t="s">
         <v>1</v>
       </c>
       <c r="I50" s="14">
@@ -2913,7 +2922,7 @@
       </c>
       <c r="M50" s="15"/>
     </row>
-    <row r="51" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" s="16" customFormat="1">
       <c r="A51" s="12" t="s">
         <v>56</v>
       </c>
@@ -2932,7 +2941,7 @@
       <c r="F51" s="14">
         <v>0.46200000000000002</v>
       </c>
-      <c r="G51" s="14" t="s">
+      <c r="G51" s="23" t="s">
         <v>1</v>
       </c>
       <c r="H51" s="14">
@@ -2954,7 +2963,7 @@
       </c>
       <c r="M51" s="15"/>
     </row>
-    <row r="52" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" s="16" customFormat="1">
       <c r="A52" s="12" t="s">
         <v>57</v>
       </c>
@@ -2994,7 +3003,7 @@
       <c r="M52" s="15"/>
       <c r="N52" s="17"/>
     </row>
-    <row r="53" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" s="16" customFormat="1">
       <c r="A53" s="12" t="s">
         <v>58</v>
       </c>
@@ -3033,7 +3042,7 @@
       </c>
       <c r="M53" s="15"/>
     </row>
-    <row r="54" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" s="16" customFormat="1">
       <c r="A54" s="12" t="s">
         <v>59</v>
       </c>
@@ -3072,7 +3081,7 @@
       </c>
       <c r="M54" s="15"/>
     </row>
-    <row r="55" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" s="16" customFormat="1">
       <c r="A55" s="12" t="s">
         <v>60</v>
       </c>
@@ -3111,7 +3120,7 @@
       </c>
       <c r="M55" s="15"/>
     </row>
-    <row r="56" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" s="16" customFormat="1">
       <c r="A56" s="12" t="s">
         <v>61</v>
       </c>
@@ -3150,7 +3159,7 @@
       </c>
       <c r="M56" s="15"/>
     </row>
-    <row r="57" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" s="16" customFormat="1">
       <c r="A57" s="12" t="s">
         <v>62</v>
       </c>
@@ -3189,7 +3198,7 @@
       </c>
       <c r="M57" s="15"/>
     </row>
-    <row r="58" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" s="16" customFormat="1">
       <c r="A58" s="12" t="s">
         <v>63</v>
       </c>
@@ -3228,7 +3237,7 @@
       </c>
       <c r="M58" s="15"/>
     </row>
-    <row r="59" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" s="16" customFormat="1">
       <c r="A59" s="12" t="s">
         <v>64</v>
       </c>
@@ -3267,7 +3276,7 @@
       </c>
       <c r="M59" s="15"/>
     </row>
-    <row r="60" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" s="16" customFormat="1">
       <c r="A60" s="12" t="s">
         <v>65</v>
       </c>
@@ -3306,7 +3315,7 @@
       </c>
       <c r="M60" s="15"/>
     </row>
-    <row r="61" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" s="16" customFormat="1">
       <c r="A61" s="12" t="s">
         <v>66</v>
       </c>
@@ -3345,7 +3354,7 @@
       </c>
       <c r="M61" s="15"/>
     </row>
-    <row r="62" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" s="16" customFormat="1">
       <c r="A62" s="12" t="s">
         <v>67</v>
       </c>
@@ -3384,7 +3393,7 @@
       </c>
       <c r="M62" s="15"/>
     </row>
-    <row r="63" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:14" s="16" customFormat="1">
       <c r="A63" s="12" t="s">
         <v>68</v>
       </c>
@@ -3403,7 +3412,7 @@
       <c r="F63" s="14">
         <v>1.6627983619020501</v>
       </c>
-      <c r="G63" s="14" t="s">
+      <c r="G63" s="23" t="s">
         <v>1</v>
       </c>
       <c r="H63" s="14">
@@ -3423,7 +3432,7 @@
       </c>
       <c r="M63" s="15"/>
     </row>
-    <row r="64" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:14" s="16" customFormat="1">
       <c r="A64" s="12" t="s">
         <v>69</v>
       </c>
@@ -3442,7 +3451,7 @@
       <c r="F64" s="14">
         <v>2.0757454835802198</v>
       </c>
-      <c r="G64" s="14" t="s">
+      <c r="G64" s="23" t="s">
         <v>1</v>
       </c>
       <c r="H64" s="14">
@@ -3462,7 +3471,7 @@
       </c>
       <c r="M64" s="15"/>
     </row>
-    <row r="65" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:14" s="16" customFormat="1">
       <c r="A65" s="18" t="s">
         <v>70</v>
       </c>
@@ -3504,7 +3513,7 @@
       <c r="M65" s="15"/>
       <c r="N65" s="22"/>
     </row>
-    <row r="66" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:14" s="16" customFormat="1">
       <c r="A66" s="18" t="s">
         <v>71</v>
       </c>
@@ -3545,7 +3554,7 @@
       </c>
       <c r="M66" s="15"/>
     </row>
-    <row r="67" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:14" s="16" customFormat="1">
       <c r="A67" s="18" t="s">
         <v>72</v>
       </c>
@@ -3586,7 +3595,7 @@
       </c>
       <c r="M67" s="15"/>
     </row>
-    <row r="68" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:14" s="16" customFormat="1">
       <c r="A68" s="18" t="s">
         <v>73</v>
       </c>
@@ -3627,7 +3636,7 @@
       </c>
       <c r="M68" s="15"/>
     </row>
-    <row r="69" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:14" s="16" customFormat="1">
       <c r="A69" s="18" t="s">
         <v>74</v>
       </c>
@@ -3668,7 +3677,7 @@
       </c>
       <c r="M69" s="15"/>
     </row>
-    <row r="70" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:14" s="16" customFormat="1">
       <c r="A70" s="18" t="s">
         <v>75</v>
       </c>
@@ -3709,7 +3718,7 @@
       </c>
       <c r="M70" s="15"/>
     </row>
-    <row r="71" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:14" s="16" customFormat="1">
       <c r="A71" s="18" t="s">
         <v>76</v>
       </c>
@@ -3750,7 +3759,7 @@
       </c>
       <c r="M71" s="15"/>
     </row>
-    <row r="72" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:14" s="16" customFormat="1">
       <c r="A72" s="18" t="s">
         <v>77</v>
       </c>
@@ -3791,7 +3800,7 @@
       </c>
       <c r="M72" s="15"/>
     </row>
-    <row r="73" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:14" s="16" customFormat="1">
       <c r="A73" s="18" t="s">
         <v>78</v>
       </c>
@@ -3832,7 +3841,7 @@
       </c>
       <c r="M73" s="15"/>
     </row>
-    <row r="74" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:14" s="16" customFormat="1">
       <c r="A74" s="18" t="s">
         <v>79</v>
       </c>
@@ -3873,7 +3882,7 @@
       </c>
       <c r="M74" s="15"/>
     </row>
-    <row r="75" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:14" s="16" customFormat="1">
       <c r="A75" s="18" t="s">
         <v>80</v>
       </c>
@@ -3914,7 +3923,7 @@
       </c>
       <c r="M75" s="15"/>
     </row>
-    <row r="76" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:14" s="16" customFormat="1">
       <c r="A76" s="18" t="s">
         <v>81</v>
       </c>
@@ -3955,7 +3964,7 @@
       </c>
       <c r="M76" s="15"/>
     </row>
-    <row r="77" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:14" s="16" customFormat="1">
       <c r="A77" s="12" t="s">
         <v>99</v>
       </c>
@@ -3996,7 +4005,7 @@
       </c>
       <c r="M77" s="15"/>
     </row>
-    <row r="78" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:14" s="16" customFormat="1">
       <c r="A78" s="12" t="s">
         <v>100</v>
       </c>
@@ -4037,7 +4046,7 @@
       </c>
       <c r="M78" s="15"/>
     </row>
-    <row r="79" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:14" s="16" customFormat="1">
       <c r="A79" s="12" t="s">
         <v>101</v>
       </c>
@@ -4078,7 +4087,7 @@
       </c>
       <c r="M79" s="15"/>
     </row>
-    <row r="80" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:14" s="16" customFormat="1">
       <c r="A80" s="18" t="s">
         <v>102</v>
       </c>
@@ -4119,7 +4128,7 @@
       </c>
       <c r="M80" s="15"/>
     </row>
-    <row r="81" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:13" s="16" customFormat="1">
       <c r="A81" s="18" t="s">
         <v>103</v>
       </c>
@@ -4160,7 +4169,7 @@
       </c>
       <c r="M81" s="15"/>
     </row>
-    <row r="82" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:13" s="16" customFormat="1">
       <c r="A82" s="18" t="s">
         <v>104</v>
       </c>
@@ -4201,7 +4210,7 @@
       </c>
       <c r="M82" s="15"/>
     </row>
-    <row r="83" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:13" s="16" customFormat="1">
       <c r="A83" s="18" t="s">
         <v>105</v>
       </c>
@@ -4242,7 +4251,7 @@
       </c>
       <c r="M83" s="15"/>
     </row>
-    <row r="84" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:13" s="16" customFormat="1">
       <c r="A84" s="18" t="s">
         <v>106</v>
       </c>
@@ -4283,7 +4292,7 @@
       </c>
       <c r="M84" s="15"/>
     </row>
-    <row r="85" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:13" s="16" customFormat="1">
       <c r="A85" s="18" t="s">
         <v>107</v>
       </c>
@@ -4324,7 +4333,7 @@
       </c>
       <c r="M85" s="15"/>
     </row>
-    <row r="86" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:13" s="16" customFormat="1">
       <c r="A86" s="18" t="s">
         <v>108</v>
       </c>
@@ -4365,7 +4374,7 @@
       </c>
       <c r="M86" s="15"/>
     </row>
-    <row r="87" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:13" s="16" customFormat="1">
       <c r="A87" s="18"/>
       <c r="B87" s="19"/>
       <c r="C87" s="20"/>
@@ -4380,7 +4389,7 @@
       <c r="L87" s="13"/>
       <c r="M87" s="15"/>
     </row>
-    <row r="88" spans="1:13" ht="18" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:13">
       <c r="A88" s="6" t="s">
         <v>88</v>
       </c>
@@ -4419,7 +4428,7 @@
       </c>
       <c r="M88" s="1"/>
     </row>
-    <row r="89" spans="1:13" ht="18" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:13">
       <c r="A89" s="6"/>
       <c r="B89" s="7"/>
       <c r="C89" s="7"/>
@@ -4434,7 +4443,7 @@
       <c r="L89" s="8"/>
       <c r="M89" s="1"/>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:13">
       <c r="A90" s="1" t="s">
         <v>91</v>
       </c>
@@ -4452,7 +4461,7 @@
       <c r="L90" s="1"/>
       <c r="M90" s="1"/>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:13">
       <c r="A91" s="1"/>
       <c r="E91" s="1"/>
       <c r="F91" s="1"/>
@@ -4464,7 +4473,7 @@
       <c r="L91" s="1"/>
       <c r="M91" s="1"/>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:13">
       <c r="A92" s="2" t="s">
         <v>2</v>
       </c>
@@ -4472,7 +4481,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:13">
       <c r="A93" s="2" t="s">
         <v>3</v>
       </c>
@@ -4480,17 +4489,17 @@
         <v>93</v>
       </c>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:13">
       <c r="A94" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:13">
       <c r="A95" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:13">
       <c r="A96" s="2" t="s">
         <v>6</v>
       </c>
@@ -4498,7 +4507,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2">
       <c r="A97" s="2" t="s">
         <v>7</v>
       </c>
@@ -4506,7 +4515,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2">
       <c r="A98" s="2" t="s">
         <v>8</v>
       </c>
@@ -4514,17 +4523,17 @@
         <v>96</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2">
       <c r="A99" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2">
       <c r="A100" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2">
       <c r="A102" s="2" t="s">
         <v>90</v>
       </c>
@@ -4532,7 +4541,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2">
       <c r="B103" t="s">
         <v>98</v>
       </c>
@@ -4556,6 +4565,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B9F749D07F25E049ABA8AD0FE40505CE" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="df84c4b9df5dab607acf25ccbb3403ac">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c7bbfe5c-3e6f-409d-9b67-9c1ca2a14071" xmlns:ns3="68868ead-3cd8-494b-9fdc-0ea8c62a0d0d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cf6d9f167100b37e85990c7a8adbe70f" ns2:_="" ns3:_="">
     <xsd:import namespace="c7bbfe5c-3e6f-409d-9b67-9c1ca2a14071"/>
@@ -4788,15 +4806,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0CA4A7A1-3616-46B0-A3CA-92ABB49C0959}">
   <ds:schemaRefs>
@@ -4815,6 +4824,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BB1C7C6-F750-45B3-9E79-150809A58FFF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6E9AC1E3-C5A1-4B99-9BCA-3A3532CACF13}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4831,12 +4848,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BB1C7C6-F750-45B3-9E79-150809A58FFF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>